<commit_message>
Updated completed lecture 3, added a few exercises
</commit_message>
<xml_diff>
--- a/misc_exercises/newton_method.xlsx
+++ b/misc_exercises/newton_method.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyhogeveen/Dropbox/Fall_2020/teaching/DSPN_Fall2020_git/misc_exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5342E3B-8F3C-4844-BE01-8315B59FD36C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7B486C-268A-4D41-A283-DC948722ACC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="7640" windowWidth="12080" windowHeight="13280" xr2:uid="{B69917CF-11E2-D148-8F5E-298E9C3D7F09}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{B69917CF-11E2-D148-8F5E-298E9C3D7F09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -483,125 +483,379 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>28561</v>
+      </c>
+      <c r="D3">
+        <f>B3^2-$C$3</f>
+        <v>-28417</v>
+      </c>
+      <c r="E3">
+        <f>2*B3</f>
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
         <f>A3+1</f>
         <v>1</v>
       </c>
+      <c r="B4">
+        <f>B3-(D3/E3)</f>
+        <v>1196.0416666666667</v>
+      </c>
+      <c r="D4">
+        <f>B4^2-$C$3</f>
+        <v>1401954.668402778</v>
+      </c>
+      <c r="E4">
+        <f>2*B4</f>
+        <v>2392.0833333333335</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
         <f t="shared" ref="A5:A22" si="0">A4+1</f>
         <v>2</v>
       </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B23" si="1">B4-(D4/E4)</f>
+        <v>609.96063476165591</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D23" si="2">B5^2-$C$3</f>
+        <v>343490.9759588422</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E23" si="3">2*B5</f>
+        <v>1219.9212695233118</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>328.39248398003832</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>79280.623534579732</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>656.78496796007664</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>207.6823164181661</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>14570.944552815265</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>415.36463283633219</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>172.6024290110052</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>1230.5985004990907</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>345.2048580220104</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>169.03759360413898</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>12.7080514780464</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>338.07518720827795</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>169.0000041803691</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1.4129647752270103E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>338.00000836073821</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <f>A22+1</f>
         <v>20</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>169.00000000000006</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>338.00000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>